<commit_message>
update ANLT600 practice test4 & COMP604 lecture
</commit_message>
<xml_diff>
--- a/Fall-Semester/ANLT600/Test4/Health data_Tai.xlsx
+++ b/Fall-Semester/ANLT600/Test4/Health data_Tai.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10916"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="1080" documentId="11_584E7FBFF7993E895E4D8452258401311C2E04FB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5CB8153-6B51-004D-9391-8F51A42DBFD1}"/>
+  <xr:revisionPtr revIDLastSave="1081" documentId="11_584E7FBFF7993E895E4D8452258401311C2E04FB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{24E6F823-14B5-EC45-A86B-96ED5326BF9E}"/>
   <bookViews>
-    <workbookView xWindow="1280" yWindow="500" windowWidth="27520" windowHeight="17500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1280" yWindow="500" windowWidth="27520" windowHeight="17500" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -410,9 +410,6 @@
     <t>r2 = 89.8%</t>
   </si>
   <si>
-    <t>increase - decrease</t>
-  </si>
-  <si>
     <t>M</t>
   </si>
   <si>
@@ -420,6 +417,9 @@
   </si>
   <si>
     <t>r2 = 0.5%</t>
+  </si>
+  <si>
+    <t>increase - lower</t>
   </si>
 </sst>
 </file>
@@ -603,7 +603,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -702,13 +702,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -16700,11 +16694,11 @@
       <c r="F3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="49">
+      <c r="G3" s="46">
         <f>AVERAGEIF($A$2:$A$41,F3,$B$2:$B$41)</f>
         <v>50.043478260869563</v>
       </c>
-      <c r="H3" s="49">
+      <c r="H3" s="46">
         <f>_xlfn.STDEV.S(N19:N41)</f>
         <v>11.683236868069351</v>
       </c>
@@ -16733,11 +16727,11 @@
       <c r="F4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="49">
+      <c r="G4" s="46">
         <f>AVERAGEIF($A$2:$A$41,F4,$B$2:$B$41)</f>
         <v>49.588235294117645</v>
       </c>
-      <c r="H4" s="49">
+      <c r="H4" s="46">
         <f>_xlfn.STDEV.S(N2:N18)</f>
         <v>17.432221686898561</v>
       </c>
@@ -17402,8 +17396,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98CA2E44-06B6-2B4E-9AF6-A645982AFFD0}">
   <dimension ref="A3:A10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -17414,7 +17408,7 @@
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="47" t="s">
         <v>116</v>
       </c>
     </row>
@@ -17430,7 +17424,7 @@
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -17453,12 +17447,12 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B3">
         <v>413.3</v>
@@ -17478,13 +17472,13 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B8" s="51" t="s">
-        <v>121</v>
+      <c r="B8" s="47" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -20954,7 +20948,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1511FC1B-BC36-4749-A836-7975098E56D6}">
   <dimension ref="A1:M82"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="81" workbookViewId="0">
+    <sheetView zoomScale="81" workbookViewId="0">
       <selection activeCell="P41" sqref="P41"/>
     </sheetView>
   </sheetViews>
@@ -23360,7 +23354,7 @@
         <v>18</v>
       </c>
       <c r="I14">
-        <f t="shared" ref="I14:I20" si="2">COUNTIF($C$2:$C$41,H14)</f>
+        <f t="shared" ref="I14:I18" si="2">COUNTIF($C$2:$C$41,H14)</f>
         <v>2</v>
       </c>
       <c r="J14">
@@ -23927,10 +23921,10 @@
       <c r="K45" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="M45" s="50">
+      <c r="M45" s="46">
         <v>49.85</v>
       </c>
-      <c r="N45" s="50">
+      <c r="N45" s="46">
         <v>14.202834675532662</v>
       </c>
     </row>
@@ -23959,10 +23953,10 @@
       <c r="K46" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="M46" s="50">
+      <c r="M46" s="46">
         <v>68.335000000000008</v>
       </c>
-      <c r="N46" s="50">
+      <c r="N46" s="46">
         <v>3.0195559191241932</v>
       </c>
     </row>
@@ -23991,10 +23985,10 @@
       <c r="K47" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="M47" s="50">
+      <c r="M47" s="46">
         <v>172.5500000000001</v>
       </c>
-      <c r="N47" s="50">
+      <c r="N47" s="46">
         <v>26.327162535667515</v>
       </c>
     </row>
@@ -24023,10 +24017,10 @@
       <c r="K48" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="M48" s="46">
+      <c r="M48">
         <v>69.400000000000006</v>
       </c>
-      <c r="N48" s="50">
+      <c r="N48" s="46">
         <v>11.297378865505458</v>
       </c>
     </row>
@@ -24055,10 +24049,10 @@
       <c r="K49" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="M49" s="50">
+      <c r="M49" s="46">
         <v>99.275000000000006</v>
       </c>
-      <c r="N49" s="50">
+      <c r="N49" s="46">
         <v>2.2869473551282731</v>
       </c>
     </row>
@@ -24087,10 +24081,10 @@
       <c r="K50" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="M50" s="50">
+      <c r="M50" s="46">
         <v>395.22500000000002</v>
       </c>
-      <c r="N50" s="50">
+      <c r="N50" s="46">
         <v>292.41176512687611</v>
       </c>
     </row>
@@ -24119,10 +24113,10 @@
       <c r="K51" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="M51" s="46">
+      <c r="M51">
         <v>7.3</v>
       </c>
-      <c r="N51" s="50">
+      <c r="N51" s="46">
         <v>4.3038444352784087</v>
       </c>
     </row>
@@ -24217,18 +24211,18 @@
       <c r="G55" s="4">
         <v>8</v>
       </c>
-      <c r="I55" s="48" t="s">
+      <c r="I55" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="J55" s="48"/>
-      <c r="L55" s="48" t="s">
+      <c r="J55" s="35"/>
+      <c r="L55" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="M55" s="48"/>
-      <c r="O55" s="48" t="s">
+      <c r="M55" s="35"/>
+      <c r="O55" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="P55" s="48"/>
+      <c r="P55" s="35"/>
     </row>
     <row r="56" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A56" s="3">
@@ -24252,12 +24246,6 @@
       <c r="G56" s="4">
         <v>7</v>
       </c>
-      <c r="I56" s="46"/>
-      <c r="J56" s="46"/>
-      <c r="L56" s="46"/>
-      <c r="M56" s="46"/>
-      <c r="O56" s="46"/>
-      <c r="P56" s="46"/>
     </row>
     <row r="57" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A57" s="3">
@@ -24281,22 +24269,22 @@
       <c r="G57" s="4">
         <v>6</v>
       </c>
-      <c r="I57" s="46" t="s">
+      <c r="I57" t="s">
         <v>50</v>
       </c>
-      <c r="J57" s="46">
+      <c r="J57">
         <v>49.85</v>
       </c>
-      <c r="L57" s="46" t="s">
+      <c r="L57" t="s">
         <v>50</v>
       </c>
-      <c r="M57" s="46">
+      <c r="M57">
         <v>68.335000000000008</v>
       </c>
-      <c r="O57" s="46" t="s">
+      <c r="O57" t="s">
         <v>50</v>
       </c>
-      <c r="P57" s="46">
+      <c r="P57">
         <v>172.5500000000001</v>
       </c>
     </row>
@@ -24322,22 +24310,22 @@
       <c r="G58" s="4">
         <v>2</v>
       </c>
-      <c r="I58" s="46" t="s">
+      <c r="I58" t="s">
         <v>51</v>
       </c>
-      <c r="J58" s="46">
+      <c r="J58">
         <v>2.2456653402750875</v>
       </c>
-      <c r="L58" s="46" t="s">
+      <c r="L58" t="s">
         <v>51</v>
       </c>
-      <c r="M58" s="46">
+      <c r="M58">
         <v>0.47743371133378165</v>
       </c>
-      <c r="O58" s="46" t="s">
+      <c r="O58" t="s">
         <v>51</v>
       </c>
-      <c r="P58" s="46">
+      <c r="P58">
         <v>4.1626898971081641</v>
       </c>
     </row>
@@ -24363,22 +24351,22 @@
       <c r="G59" s="4">
         <v>11</v>
       </c>
-      <c r="I59" s="46" t="s">
+      <c r="I59" t="s">
         <v>52</v>
       </c>
-      <c r="J59" s="46">
+      <c r="J59">
         <v>49.5</v>
       </c>
-      <c r="L59" s="46" t="s">
+      <c r="L59" t="s">
         <v>52</v>
       </c>
-      <c r="M59" s="46">
+      <c r="M59">
         <v>68.3</v>
       </c>
-      <c r="O59" s="46" t="s">
+      <c r="O59" t="s">
         <v>52</v>
       </c>
-      <c r="P59" s="46">
+      <c r="P59">
         <v>169.95</v>
       </c>
     </row>
@@ -24404,22 +24392,22 @@
       <c r="G60" s="4">
         <v>9</v>
       </c>
-      <c r="I60" s="46" t="s">
+      <c r="I60" t="s">
         <v>53</v>
       </c>
-      <c r="J60" s="46">
+      <c r="J60">
         <v>68</v>
       </c>
-      <c r="L60" s="46" t="s">
+      <c r="L60" t="s">
         <v>53</v>
       </c>
-      <c r="M60" s="46">
+      <c r="M60">
         <v>68.3</v>
       </c>
-      <c r="O60" s="46" t="s">
+      <c r="O60" t="s">
         <v>53</v>
       </c>
-      <c r="P60" s="46" t="e">
+      <c r="P60" t="e">
         <v>#N/A</v>
       </c>
     </row>
@@ -24445,22 +24433,22 @@
       <c r="G61" s="4">
         <v>7</v>
       </c>
-      <c r="I61" s="46" t="s">
+      <c r="I61" t="s">
         <v>54</v>
       </c>
-      <c r="J61" s="46">
+      <c r="J61">
         <v>14.202834675532662</v>
       </c>
-      <c r="L61" s="46" t="s">
+      <c r="L61" t="s">
         <v>54</v>
       </c>
-      <c r="M61" s="46">
+      <c r="M61">
         <v>3.0195559191241932</v>
       </c>
-      <c r="O61" s="46" t="s">
+      <c r="O61" t="s">
         <v>54</v>
       </c>
-      <c r="P61" s="46">
+      <c r="P61">
         <v>26.327162535667515</v>
       </c>
     </row>
@@ -24486,22 +24474,22 @@
       <c r="G62" s="4">
         <v>5</v>
       </c>
-      <c r="I62" s="46" t="s">
+      <c r="I62" t="s">
         <v>55</v>
       </c>
-      <c r="J62" s="46">
+      <c r="J62">
         <v>201.72051282051297</v>
       </c>
-      <c r="L62" s="46" t="s">
+      <c r="L62" t="s">
         <v>55</v>
       </c>
-      <c r="M62" s="46">
+      <c r="M62">
         <v>9.1177179487179512</v>
       </c>
-      <c r="O62" s="46" t="s">
+      <c r="O62" t="s">
         <v>55</v>
       </c>
-      <c r="P62" s="46">
+      <c r="P62">
         <v>693.11948717945518</v>
       </c>
     </row>
@@ -24527,22 +24515,22 @@
       <c r="G63" s="4">
         <v>4</v>
       </c>
-      <c r="I63" s="46" t="s">
+      <c r="I63" t="s">
         <v>56</v>
       </c>
-      <c r="J63" s="46">
+      <c r="J63">
         <v>-0.62992781792904484</v>
       </c>
-      <c r="L63" s="46" t="s">
+      <c r="L63" t="s">
         <v>56</v>
       </c>
-      <c r="M63" s="46">
+      <c r="M63">
         <v>0.50555863073135576</v>
       </c>
-      <c r="O63" s="46" t="s">
+      <c r="O63" t="s">
         <v>56</v>
       </c>
-      <c r="P63" s="46">
+      <c r="P63">
         <v>-0.16641631736650631</v>
       </c>
     </row>
@@ -24568,22 +24556,22 @@
       <c r="G64" s="4">
         <v>2</v>
       </c>
-      <c r="I64" s="46" t="s">
+      <c r="I64" t="s">
         <v>57</v>
       </c>
-      <c r="J64" s="46">
+      <c r="J64">
         <v>-2.079796525781499E-2</v>
       </c>
-      <c r="L64" s="46" t="s">
+      <c r="L64" t="s">
         <v>57</v>
       </c>
-      <c r="M64" s="46">
+      <c r="M64">
         <v>4.5652331555308429E-2</v>
       </c>
-      <c r="O64" s="46" t="s">
+      <c r="O64" t="s">
         <v>57</v>
       </c>
-      <c r="P64" s="46">
+      <c r="P64">
         <v>0.37037477969411386</v>
       </c>
     </row>
@@ -24609,22 +24597,22 @@
       <c r="G65" s="4">
         <v>1</v>
       </c>
-      <c r="I65" s="46" t="s">
+      <c r="I65" t="s">
         <v>58</v>
       </c>
-      <c r="J65" s="46">
+      <c r="J65">
         <v>57</v>
       </c>
-      <c r="L65" s="46" t="s">
+      <c r="L65" t="s">
         <v>58</v>
       </c>
-      <c r="M65" s="46">
+      <c r="M65">
         <v>14.900000000000006</v>
       </c>
-      <c r="O65" s="46" t="s">
+      <c r="O65" t="s">
         <v>58</v>
       </c>
-      <c r="P65" s="46">
+      <c r="P65">
         <v>117.6</v>
       </c>
     </row>
@@ -24650,22 +24638,22 @@
       <c r="G66" s="4">
         <v>1</v>
       </c>
-      <c r="I66" s="46" t="s">
+      <c r="I66" t="s">
         <v>59</v>
       </c>
-      <c r="J66" s="46">
+      <c r="J66">
         <v>20</v>
       </c>
-      <c r="L66" s="46" t="s">
+      <c r="L66" t="s">
         <v>59</v>
       </c>
-      <c r="M66" s="46">
+      <c r="M66">
         <v>61.3</v>
       </c>
-      <c r="O66" s="46" t="s">
+      <c r="O66" t="s">
         <v>59</v>
       </c>
-      <c r="P66" s="46">
+      <c r="P66">
         <v>119.5</v>
       </c>
     </row>
@@ -24691,22 +24679,22 @@
       <c r="G67" s="4">
         <v>14</v>
       </c>
-      <c r="I67" s="46" t="s">
+      <c r="I67" t="s">
         <v>60</v>
       </c>
-      <c r="J67" s="46">
+      <c r="J67">
         <v>77</v>
       </c>
-      <c r="L67" s="46" t="s">
+      <c r="L67" t="s">
         <v>60</v>
       </c>
-      <c r="M67" s="46">
+      <c r="M67">
         <v>76.2</v>
       </c>
-      <c r="O67" s="46" t="s">
+      <c r="O67" t="s">
         <v>60</v>
       </c>
-      <c r="P67" s="46">
+      <c r="P67">
         <v>237.1</v>
       </c>
     </row>
@@ -24732,22 +24720,22 @@
       <c r="G68" s="4">
         <v>12</v>
       </c>
-      <c r="I68" s="46" t="s">
+      <c r="I68" t="s">
         <v>61</v>
       </c>
-      <c r="J68" s="46">
+      <c r="J68">
         <v>1994</v>
       </c>
-      <c r="L68" s="46" t="s">
+      <c r="L68" t="s">
         <v>61</v>
       </c>
-      <c r="M68" s="46">
+      <c r="M68">
         <v>2733.4</v>
       </c>
-      <c r="O68" s="46" t="s">
+      <c r="O68" t="s">
         <v>61</v>
       </c>
-      <c r="P68" s="46">
+      <c r="P68">
         <v>6902.0000000000036</v>
       </c>
     </row>
@@ -24773,22 +24761,22 @@
       <c r="G69" s="4">
         <v>11</v>
       </c>
-      <c r="I69" s="47" t="s">
+      <c r="I69" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="J69" s="47">
+      <c r="J69" s="33">
         <v>40</v>
       </c>
-      <c r="L69" s="47" t="s">
+      <c r="L69" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="M69" s="47">
+      <c r="M69" s="33">
         <v>40</v>
       </c>
-      <c r="O69" s="47" t="s">
+      <c r="O69" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="P69" s="47">
+      <c r="P69" s="33">
         <v>40</v>
       </c>
     </row>
@@ -24892,22 +24880,22 @@
       <c r="G73" s="4">
         <v>7</v>
       </c>
-      <c r="I73" s="48" t="s">
+      <c r="I73" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="J73" s="48"/>
-      <c r="L73" s="48" t="s">
+      <c r="J73" s="35"/>
+      <c r="L73" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="M73" s="48"/>
-      <c r="O73" s="48" t="s">
+      <c r="M73" s="35"/>
+      <c r="O73" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="P73" s="48"/>
-      <c r="R73" s="48" t="s">
+      <c r="P73" s="35"/>
+      <c r="R73" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="S73" s="48"/>
+      <c r="S73" s="35"/>
     </row>
     <row r="74" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A74" s="3">
@@ -24931,14 +24919,6 @@
       <c r="G74" s="4">
         <v>6</v>
       </c>
-      <c r="I74" s="46"/>
-      <c r="J74" s="46"/>
-      <c r="L74" s="46"/>
-      <c r="M74" s="46"/>
-      <c r="O74" s="46"/>
-      <c r="P74" s="46"/>
-      <c r="R74" s="46"/>
-      <c r="S74" s="46"/>
     </row>
     <row r="75" spans="1:19" ht="18" x14ac:dyDescent="0.2">
       <c r="A75" s="3">
@@ -24962,28 +24942,28 @@
       <c r="G75" s="4">
         <v>2</v>
       </c>
-      <c r="I75" s="46" t="s">
+      <c r="I75" t="s">
         <v>50</v>
       </c>
-      <c r="J75" s="46">
+      <c r="J75">
         <v>69.400000000000006</v>
       </c>
-      <c r="L75" s="46" t="s">
+      <c r="L75" t="s">
         <v>50</v>
       </c>
-      <c r="M75" s="46">
+      <c r="M75">
         <v>99.275000000000006</v>
       </c>
-      <c r="O75" s="46" t="s">
+      <c r="O75" t="s">
         <v>50</v>
       </c>
-      <c r="P75" s="46">
+      <c r="P75">
         <v>395.22500000000002</v>
       </c>
-      <c r="R75" s="46" t="s">
+      <c r="R75" t="s">
         <v>50</v>
       </c>
-      <c r="S75" s="46">
+      <c r="S75">
         <v>7.3</v>
       </c>
     </row>
@@ -25009,28 +24989,28 @@
       <c r="G76" s="4">
         <v>2</v>
       </c>
-      <c r="I76" s="46" t="s">
+      <c r="I76" t="s">
         <v>51</v>
       </c>
-      <c r="J76" s="46">
+      <c r="J76">
         <v>1.7862724402423149</v>
       </c>
-      <c r="L76" s="46" t="s">
+      <c r="L76" t="s">
         <v>51</v>
       </c>
-      <c r="M76" s="46">
+      <c r="M76">
         <v>0.36159812655516493</v>
       </c>
-      <c r="O76" s="46" t="s">
+      <c r="O76" t="s">
         <v>51</v>
       </c>
-      <c r="P76" s="46">
+      <c r="P76">
         <v>46.234359621556173</v>
       </c>
-      <c r="R76" s="46" t="s">
+      <c r="R76" t="s">
         <v>51</v>
       </c>
-      <c r="S76" s="46">
+      <c r="S76">
         <v>0.68049755552604529</v>
       </c>
     </row>
@@ -25056,28 +25036,28 @@
       <c r="G77" s="4">
         <v>0</v>
       </c>
-      <c r="I77" s="46" t="s">
+      <c r="I77" t="s">
         <v>52</v>
       </c>
-      <c r="J77" s="46">
+      <c r="J77">
         <v>66</v>
       </c>
-      <c r="L77" s="46" t="s">
+      <c r="L77" t="s">
         <v>52</v>
       </c>
-      <c r="M77" s="46">
+      <c r="M77">
         <v>99</v>
       </c>
-      <c r="O77" s="46" t="s">
+      <c r="O77" t="s">
         <v>52</v>
       </c>
-      <c r="P77" s="46">
+      <c r="P77">
         <v>282.5</v>
       </c>
-      <c r="R77" s="46" t="s">
+      <c r="R77" t="s">
         <v>52</v>
       </c>
-      <c r="S77" s="46">
+      <c r="S77">
         <v>8</v>
       </c>
     </row>
@@ -25103,28 +25083,28 @@
       <c r="G78" s="4">
         <v>0</v>
       </c>
-      <c r="I78" s="46" t="s">
+      <c r="I78" t="s">
         <v>53</v>
       </c>
-      <c r="J78" s="46">
+      <c r="J78">
         <v>64</v>
       </c>
-      <c r="L78" s="46" t="s">
+      <c r="L78" t="s">
         <v>53</v>
       </c>
-      <c r="M78" s="46">
+      <c r="M78">
         <v>101</v>
       </c>
-      <c r="O78" s="46" t="s">
+      <c r="O78" t="s">
         <v>53</v>
       </c>
-      <c r="P78" s="46">
+      <c r="P78">
         <v>265</v>
       </c>
-      <c r="R78" s="46" t="s">
+      <c r="R78" t="s">
         <v>53</v>
       </c>
-      <c r="S78" s="46">
+      <c r="S78">
         <v>8</v>
       </c>
     </row>
@@ -25150,28 +25130,28 @@
       <c r="G79" s="4">
         <v>11</v>
       </c>
-      <c r="I79" s="46" t="s">
+      <c r="I79" t="s">
         <v>54</v>
       </c>
-      <c r="J79" s="46">
+      <c r="J79">
         <v>11.297378865505458</v>
       </c>
-      <c r="L79" s="46" t="s">
+      <c r="L79" t="s">
         <v>54</v>
       </c>
-      <c r="M79" s="46">
+      <c r="M79">
         <v>2.2869473551282731</v>
       </c>
-      <c r="O79" s="46" t="s">
+      <c r="O79" t="s">
         <v>54</v>
       </c>
-      <c r="P79" s="46">
+      <c r="P79">
         <v>292.41176512687611</v>
       </c>
-      <c r="R79" s="46" t="s">
+      <c r="R79" t="s">
         <v>54</v>
       </c>
-      <c r="S79" s="46">
+      <c r="S79">
         <v>4.3038444352784087</v>
       </c>
     </row>
@@ -25197,28 +25177,28 @@
       <c r="G80" s="4">
         <v>8</v>
       </c>
-      <c r="I80" s="46" t="s">
+      <c r="I80" t="s">
         <v>55</v>
       </c>
-      <c r="J80" s="46">
+      <c r="J80">
         <v>127.63076923076937</v>
       </c>
-      <c r="L80" s="46" t="s">
+      <c r="L80" t="s">
         <v>55</v>
       </c>
-      <c r="M80" s="46">
+      <c r="M80">
         <v>5.2301282051282039</v>
       </c>
-      <c r="O80" s="46" t="s">
+      <c r="O80" t="s">
         <v>55</v>
       </c>
-      <c r="P80" s="46">
+      <c r="P80">
         <v>85504.64038461537</v>
       </c>
-      <c r="R80" s="46" t="s">
+      <c r="R80" t="s">
         <v>55</v>
       </c>
-      <c r="S80" s="46">
+      <c r="S80">
         <v>18.523076923076925</v>
       </c>
     </row>
@@ -25244,28 +25224,28 @@
       <c r="G81" s="4">
         <v>7</v>
       </c>
-      <c r="I81" s="46" t="s">
+      <c r="I81" t="s">
         <v>56</v>
       </c>
-      <c r="J81" s="46">
+      <c r="J81">
         <v>-0.6395175820074841</v>
       </c>
-      <c r="L81" s="46" t="s">
+      <c r="L81" t="s">
         <v>56</v>
       </c>
-      <c r="M81" s="46">
+      <c r="M81">
         <v>-1.1872729824270762</v>
       </c>
-      <c r="O81" s="46" t="s">
+      <c r="O81" t="s">
         <v>56</v>
       </c>
-      <c r="P81" s="46">
+      <c r="P81">
         <v>0.47143125149810761</v>
       </c>
-      <c r="R81" s="46" t="s">
+      <c r="R81" t="s">
         <v>56</v>
       </c>
-      <c r="S81" s="46">
+      <c r="S81">
         <v>-1.1479706940548411</v>
       </c>
     </row>
@@ -25291,28 +25271,28 @@
       <c r="G82" s="4">
         <v>3</v>
       </c>
-      <c r="I82" s="46" t="s">
+      <c r="I82" t="s">
         <v>57</v>
       </c>
-      <c r="J82" s="46">
+      <c r="J82">
         <v>0.68002365789764041</v>
       </c>
-      <c r="L82" s="46" t="s">
+      <c r="L82" t="s">
         <v>57</v>
       </c>
-      <c r="M82" s="46">
+      <c r="M82">
         <v>9.001061157007044E-2</v>
       </c>
-      <c r="O82" s="46" t="s">
+      <c r="O82" t="s">
         <v>57</v>
       </c>
-      <c r="P82" s="46">
+      <c r="P82">
         <v>0.96657635197114089</v>
       </c>
-      <c r="R82" s="46" t="s">
+      <c r="R82" t="s">
         <v>57</v>
       </c>
-      <c r="S82" s="46">
+      <c r="S82">
         <v>-0.13923148100207461</v>
       </c>
     </row>
@@ -25338,28 +25318,28 @@
       <c r="G83" s="4">
         <v>3</v>
       </c>
-      <c r="I83" s="46" t="s">
+      <c r="I83" t="s">
         <v>58</v>
       </c>
-      <c r="J83" s="46">
+      <c r="J83">
         <v>40</v>
       </c>
-      <c r="L83" s="46" t="s">
+      <c r="L83" t="s">
         <v>58</v>
       </c>
-      <c r="M83" s="46">
+      <c r="M83">
         <v>7</v>
       </c>
-      <c r="O83" s="46" t="s">
+      <c r="O83" t="s">
         <v>58</v>
       </c>
-      <c r="P83" s="46">
+      <c r="P83">
         <v>1221</v>
       </c>
-      <c r="R83" s="46" t="s">
+      <c r="R83" t="s">
         <v>58</v>
       </c>
-      <c r="S83" s="46">
+      <c r="S83">
         <v>14</v>
       </c>
     </row>
@@ -25385,106 +25365,106 @@
       <c r="G84" s="4">
         <v>2</v>
       </c>
-      <c r="I84" s="46" t="s">
+      <c r="I84" t="s">
         <v>59</v>
       </c>
-      <c r="J84" s="46">
+      <c r="J84">
         <v>56</v>
       </c>
-      <c r="L84" s="46" t="s">
+      <c r="L84" t="s">
         <v>59</v>
       </c>
-      <c r="M84" s="46">
+      <c r="M84">
         <v>96</v>
       </c>
-      <c r="O84" s="46" t="s">
+      <c r="O84" t="s">
         <v>59</v>
       </c>
-      <c r="P84" s="46">
+      <c r="P84">
         <v>31</v>
       </c>
-      <c r="R84" s="46" t="s">
+      <c r="R84" t="s">
         <v>59</v>
       </c>
-      <c r="S84" s="46">
+      <c r="S84">
         <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="I85" s="46" t="s">
+      <c r="I85" t="s">
         <v>60</v>
       </c>
-      <c r="J85" s="46">
+      <c r="J85">
         <v>96</v>
       </c>
-      <c r="L85" s="46" t="s">
+      <c r="L85" t="s">
         <v>60</v>
       </c>
-      <c r="M85" s="46">
+      <c r="M85">
         <v>103</v>
       </c>
-      <c r="O85" s="46" t="s">
+      <c r="O85" t="s">
         <v>60</v>
       </c>
-      <c r="P85" s="46">
+      <c r="P85">
         <v>1252</v>
       </c>
-      <c r="R85" s="46" t="s">
+      <c r="R85" t="s">
         <v>60</v>
       </c>
-      <c r="S85" s="46">
+      <c r="S85">
         <v>14</v>
       </c>
     </row>
     <row r="86" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="I86" s="46" t="s">
+      <c r="I86" t="s">
         <v>61</v>
       </c>
-      <c r="J86" s="46">
+      <c r="J86">
         <v>2776</v>
       </c>
-      <c r="L86" s="46" t="s">
+      <c r="L86" t="s">
         <v>61</v>
       </c>
-      <c r="M86" s="46">
+      <c r="M86">
         <v>3971</v>
       </c>
-      <c r="O86" s="46" t="s">
+      <c r="O86" t="s">
         <v>61</v>
       </c>
-      <c r="P86" s="46">
+      <c r="P86">
         <v>15809</v>
       </c>
-      <c r="R86" s="46" t="s">
+      <c r="R86" t="s">
         <v>61</v>
       </c>
-      <c r="S86" s="46">
+      <c r="S86">
         <v>292</v>
       </c>
     </row>
     <row r="87" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="I87" s="47" t="s">
+      <c r="I87" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="J87" s="47">
+      <c r="J87" s="33">
         <v>40</v>
       </c>
-      <c r="L87" s="47" t="s">
+      <c r="L87" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="M87" s="47">
+      <c r="M87" s="33">
         <v>40</v>
       </c>
-      <c r="O87" s="47" t="s">
+      <c r="O87" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="P87" s="47">
+      <c r="P87" s="33">
         <v>40</v>
       </c>
-      <c r="R87" s="47" t="s">
+      <c r="R87" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="S87" s="47">
+      <c r="S87" s="33">
         <v>40</v>
       </c>
     </row>

</xml_diff>